<commit_message>
Generating multiple Word documents
</commit_message>
<xml_diff>
--- a/test-sheet.xlsx
+++ b/test-sheet.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Col name 1</t>
-  </si>
-  <si>
-    <t>Col name 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
   <si>
     <t>cell1</t>
   </si>
@@ -34,6 +28,54 @@
   </si>
   <si>
     <t>cell4</t>
+  </si>
+  <si>
+    <t>Colname 1</t>
+  </si>
+  <si>
+    <t>Colname 2</t>
+  </si>
+  <si>
+    <t>cell5</t>
+  </si>
+  <si>
+    <t>cell7</t>
+  </si>
+  <si>
+    <t>cell9</t>
+  </si>
+  <si>
+    <t>cell11</t>
+  </si>
+  <si>
+    <t>cell13</t>
+  </si>
+  <si>
+    <t>cell6</t>
+  </si>
+  <si>
+    <t>cell8</t>
+  </si>
+  <si>
+    <t>cell10</t>
+  </si>
+  <si>
+    <t>cell12</t>
+  </si>
+  <si>
+    <t>cell14</t>
+  </si>
+  <si>
+    <t>Colname 3</t>
+  </si>
+  <si>
+    <t>Colname 4</t>
+  </si>
+  <si>
+    <t>Colname 5</t>
+  </si>
+  <si>
+    <t>Colname 6</t>
   </si>
 </sst>
 </file>
@@ -372,36 +414,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>